<commit_message>
Graph à 8 cm de haut
</commit_message>
<xml_diff>
--- a/bench/Bench.xlsx
+++ b/bench/Bench.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions non exécutées" sheetId="1" r:id="rId1"/>
@@ -12648,8 +12648,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>251738</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>189074</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>51074</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12673,13 +12673,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>409574</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>38098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>323174</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>8099</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>60598</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12713,8 +12713,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>327937</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>131925</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>184425</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12743,8 +12743,8 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>61237</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>174900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12778,8 +12778,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>275550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>141450</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12808,8 +12808,8 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>299362</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>150975</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>12975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13154,7 +13154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -21941,8 +21941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>